<commit_message>
Added lit sources and some lines to createlatestmodel
</commit_message>
<xml_diff>
--- a/isoenzymes.xlsx
+++ b/isoenzymes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="8595" windowHeight="4935" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="48" windowWidth="8592" windowHeight="4932" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -881,7 +881,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -889,13 +889,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -910,8 +923,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1217,7 +1232,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1229,7 +1244,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1241,7 +1256,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1251,19 +1266,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="3" width="64.85546875" customWidth="1"/>
-    <col min="4" max="4" width="146.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="64.88671875" customWidth="1"/>
+    <col min="4" max="4" width="146.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>282</v>
       </c>
@@ -1277,7 +1292,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1291,7 +1306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1305,7 +1320,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1319,7 +1334,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1333,7 +1348,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1347,7 +1362,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1361,21 +1376,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1389,7 +1404,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1403,7 +1418,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1417,7 +1432,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1431,7 +1446,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1445,21 +1460,21 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1473,7 +1488,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1487,7 +1502,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1501,7 +1516,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1515,7 +1530,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -1529,7 +1544,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -1543,7 +1558,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -1557,7 +1572,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -1571,7 +1586,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -1585,7 +1600,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -1599,7 +1614,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -1613,7 +1628,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>89</v>
       </c>
@@ -1627,7 +1642,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1641,7 +1656,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>96</v>
       </c>
@@ -1655,7 +1670,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>100</v>
       </c>
@@ -1669,7 +1684,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>104</v>
       </c>
@@ -1683,7 +1698,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>108</v>
       </c>
@@ -1697,7 +1712,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -1711,7 +1726,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -1725,7 +1740,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>120</v>
       </c>
@@ -1739,7 +1754,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>124</v>
       </c>
@@ -1753,7 +1768,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>128</v>
       </c>
@@ -1767,7 +1782,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>132</v>
       </c>
@@ -1781,7 +1796,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>136</v>
       </c>
@@ -1795,7 +1810,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>140</v>
       </c>
@@ -1809,7 +1824,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>144</v>
       </c>
@@ -1823,7 +1838,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -1837,7 +1852,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>152</v>
       </c>
@@ -1851,7 +1866,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>156</v>
       </c>
@@ -1865,7 +1880,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>160</v>
       </c>
@@ -1879,7 +1894,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>164</v>
       </c>
@@ -1893,7 +1908,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>168</v>
       </c>
@@ -1907,7 +1922,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>171</v>
       </c>
@@ -1921,7 +1936,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>175</v>
       </c>
@@ -1935,7 +1950,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>179</v>
       </c>
@@ -1949,7 +1964,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>183</v>
       </c>
@@ -1963,7 +1978,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>187</v>
       </c>
@@ -1977,7 +1992,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>191</v>
       </c>
@@ -1991,7 +2006,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>195</v>
       </c>
@@ -2005,7 +2020,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>199</v>
       </c>
@@ -2019,7 +2034,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>203</v>
       </c>
@@ -2033,7 +2048,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>207</v>
       </c>
@@ -2047,7 +2062,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>209</v>
       </c>
@@ -2061,7 +2076,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>213</v>
       </c>
@@ -2075,7 +2090,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>216</v>
       </c>
@@ -2089,7 +2104,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>220</v>
       </c>
@@ -2103,7 +2118,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>223</v>
       </c>
@@ -2117,7 +2132,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>227</v>
       </c>
@@ -2131,7 +2146,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>230</v>
       </c>
@@ -2145,7 +2160,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>234</v>
       </c>
@@ -2159,7 +2174,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>237</v>
       </c>
@@ -2173,7 +2188,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>240</v>
       </c>
@@ -2187,7 +2202,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>242</v>
       </c>
@@ -2201,7 +2216,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>244</v>
       </c>
@@ -2215,7 +2230,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>246</v>
       </c>
@@ -2229,7 +2244,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>248</v>
       </c>
@@ -2243,7 +2258,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>250</v>
       </c>
@@ -2257,7 +2272,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>252</v>
       </c>
@@ -2271,7 +2286,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>254</v>
       </c>
@@ -2285,7 +2300,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>256</v>
       </c>
@@ -2299,7 +2314,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>258</v>
       </c>
@@ -2313,7 +2328,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>260</v>
       </c>
@@ -2327,7 +2342,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>262</v>
       </c>
@@ -2341,7 +2356,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>264</v>
       </c>
@@ -2355,7 +2370,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>266</v>
       </c>
@@ -2369,7 +2384,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>269</v>
       </c>
@@ -2383,7 +2398,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>272</v>
       </c>
@@ -2397,7 +2412,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>275</v>
       </c>
@@ -2411,7 +2426,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>278</v>
       </c>

</xml_diff>